<commit_message>
Added more llava trials
</commit_message>
<xml_diff>
--- a/llava-trials.xlsx
+++ b/llava-trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryana\OneDrive\Documents\Actual Documents\extracted_frames_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460AAF6B-B260-41BB-9B89-C6F65DD65ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32D50D8-5FFF-45DB-9D9F-77D3C9BE0AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{AD63279E-0698-49CC-BCD4-922352F5CF60}"/>
   </bookViews>
@@ -1358,15 +1358,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1393,14 +1385,10 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0B23B55E-9F11-4D0C-B41D-B78DF39C4D66}" name="Table1" displayName="Table1" ref="A1:M201" totalsRowShown="0">
-  <autoFilter ref="A1:M201" xr:uid="{0B23B55E-9F11-4D0C-B41D-B78DF39C4D66}">
-    <filterColumn colId="0">
-      <colorFilter dxfId="0"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M201" xr:uid="{0B23B55E-9F11-4D0C-B41D-B78DF39C4D66}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{780E54EF-E4C8-472D-B38F-6EF20FD49788}" name="Trial" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{FD2CDD26-7F8C-42B7-A892-6E8BF10FD686}" name="Number of vehicles in accident" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{780E54EF-E4C8-472D-B38F-6EF20FD49788}" name="Trial" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{FD2CDD26-7F8C-42B7-A892-6E8BF10FD686}" name="Number of vehicles in accident" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{28840B24-D802-4E51-B3D8-A4AC3141C086}" name="Accident Type"/>
     <tableColumn id="4" xr3:uid="{35075EFF-1D87-49F5-93E9-59D271CDDC06}" name="Person Injury? "/>
     <tableColumn id="5" xr3:uid="{1F1E646D-6596-493A-B8FC-87B63480C50A}" name="Need for ambulance?"/>
@@ -1411,7 +1399,7 @@
     <tableColumn id="10" xr3:uid="{0FADADE6-DAC9-4A65-83C6-17E454613E96}" name="Weather"/>
     <tableColumn id="11" xr3:uid="{B735971A-27A7-4893-8554-C56AB220D259}" name="Low Res/Bad Footage?"/>
     <tableColumn id="12" xr3:uid="{24E21628-77B2-42DF-B7FD-48341EB9586F}" name="Other"/>
-    <tableColumn id="13" xr3:uid="{84B52FAF-C748-46A6-8894-E0B9B6C6D109}" name="Color" dataDxfId="1">
+    <tableColumn id="13" xr3:uid="{84B52FAF-C748-46A6-8894-E0B9B6C6D109}" name="Color" dataDxfId="0">
       <calculatedColumnFormula array="1">GetColor</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1738,8 +1726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F41316-F566-4B06-BB05-B7BBB865FBE7}">
   <dimension ref="A1:M213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C211" sqref="C211"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="N180" sqref="N180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1785,7 +1773,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1827,7 +1815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -1860,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1902,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -1938,7 +1926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1980,7 +1968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -2016,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -2058,7 +2046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
@@ -2097,7 +2085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>5</v>
       </c>
@@ -2139,7 +2127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
@@ -2175,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>6</v>
       </c>
@@ -2217,7 +2205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
@@ -2256,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>7</v>
       </c>
@@ -2298,7 +2286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -2337,7 +2325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>8</v>
       </c>
@@ -2379,7 +2367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>49</v>
       </c>
@@ -2418,7 +2406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>9</v>
       </c>
@@ -2460,7 +2448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>54</v>
       </c>
@@ -2496,7 +2484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>10</v>
       </c>
@@ -2535,7 +2523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>57</v>
       </c>
@@ -2571,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>11</v>
       </c>
@@ -2649,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>12</v>
       </c>
@@ -2691,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>63</v>
       </c>
@@ -2727,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>13</v>
       </c>
@@ -2808,7 +2796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>14</v>
       </c>
@@ -2850,7 +2838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>71</v>
       </c>
@@ -2886,7 +2874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>15</v>
       </c>
@@ -2928,7 +2916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>74</v>
       </c>
@@ -2964,7 +2952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>16</v>
       </c>
@@ -3006,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>77</v>
       </c>
@@ -3042,7 +3030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>17</v>
       </c>
@@ -3084,7 +3072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>82</v>
       </c>
@@ -3120,7 +3108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>18</v>
       </c>
@@ -3162,7 +3150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>85</v>
       </c>
@@ -3198,7 +3186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>19</v>
       </c>
@@ -3240,7 +3228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>87</v>
       </c>
@@ -3276,7 +3264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>20</v>
       </c>
@@ -3357,7 +3345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>21</v>
       </c>
@@ -3396,7 +3384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>92</v>
       </c>
@@ -3435,7 +3423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>22</v>
       </c>
@@ -3477,7 +3465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>94</v>
       </c>
@@ -3516,7 +3504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>23</v>
       </c>
@@ -3558,7 +3546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>98</v>
       </c>
@@ -3594,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>24</v>
       </c>
@@ -3636,7 +3624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>100</v>
       </c>
@@ -3672,7 +3660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>25</v>
       </c>
@@ -3714,7 +3702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>102</v>
       </c>
@@ -3750,7 +3738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>26</v>
       </c>
@@ -3828,7 +3816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>27</v>
       </c>
@@ -3870,7 +3858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>112</v>
       </c>
@@ -3906,7 +3894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>28</v>
       </c>
@@ -3948,7 +3936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>115</v>
       </c>
@@ -3987,7 +3975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>29</v>
       </c>
@@ -4029,7 +4017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>120</v>
       </c>
@@ -4065,7 +4053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>30</v>
       </c>
@@ -4107,7 +4095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>124</v>
       </c>
@@ -4143,7 +4131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>31</v>
       </c>
@@ -4196,7 +4184,7 @@
         <v>141</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>117</v>
+        <v>14</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>14</v>
@@ -4221,7 +4209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>32</v>
       </c>
@@ -4303,7 +4291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>33</v>
       </c>
@@ -4345,7 +4333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>137</v>
       </c>
@@ -4384,7 +4372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>34</v>
       </c>
@@ -4426,7 +4414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>140</v>
       </c>
@@ -4462,7 +4450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>35</v>
       </c>
@@ -4504,7 +4492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>144</v>
       </c>
@@ -4540,7 +4528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>36</v>
       </c>
@@ -4582,7 +4570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>147</v>
       </c>
@@ -4618,7 +4606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>37</v>
       </c>
@@ -4660,7 +4648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>150</v>
       </c>
@@ -4699,7 +4687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>38</v>
       </c>
@@ -4741,7 +4729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>155</v>
       </c>
@@ -4780,7 +4768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>39</v>
       </c>
@@ -4822,7 +4810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>158</v>
       </c>
@@ -4855,7 +4843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>40</v>
       </c>
@@ -4897,7 +4885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>161</v>
       </c>
@@ -4933,7 +4921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>41</v>
       </c>
@@ -4975,7 +4963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>164</v>
       </c>
@@ -5011,7 +4999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>42</v>
       </c>
@@ -5053,7 +5041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>168</v>
       </c>
@@ -5089,7 +5077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>43</v>
       </c>
@@ -5131,7 +5119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>171</v>
       </c>
@@ -5167,7 +5155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>44</v>
       </c>
@@ -5209,7 +5197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>175</v>
       </c>
@@ -5245,7 +5233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>45</v>
       </c>
@@ -5287,7 +5275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>179</v>
       </c>
@@ -5323,7 +5311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>46</v>
       </c>
@@ -5365,7 +5353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>183</v>
       </c>
@@ -5401,7 +5389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>47</v>
       </c>
@@ -5443,7 +5431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>185</v>
       </c>
@@ -5479,7 +5467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>48</v>
       </c>
@@ -5521,7 +5509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>188</v>
       </c>
@@ -5557,7 +5545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>49</v>
       </c>
@@ -5599,7 +5587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>191</v>
       </c>
@@ -5638,7 +5626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>50</v>
       </c>
@@ -5716,7 +5704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>51</v>
       </c>
@@ -5794,7 +5782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>52</v>
       </c>
@@ -5836,7 +5824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>203</v>
       </c>
@@ -5872,7 +5860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>53</v>
       </c>
@@ -5953,7 +5941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>54</v>
       </c>
@@ -5995,7 +5983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
         <v>210</v>
       </c>
@@ -6037,7 +6025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>55</v>
       </c>
@@ -6115,7 +6103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <v>56</v>
       </c>
@@ -6157,7 +6145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>215</v>
       </c>
@@ -6196,7 +6184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <v>57</v>
       </c>
@@ -6274,7 +6262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>58</v>
       </c>
@@ -6316,7 +6304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>221</v>
       </c>
@@ -6355,7 +6343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="5">
         <v>59</v>
       </c>
@@ -6397,7 +6385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>222</v>
       </c>
@@ -6433,7 +6421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <v>60</v>
       </c>
@@ -6475,7 +6463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>224</v>
       </c>
@@ -6511,7 +6499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>61</v>
       </c>
@@ -6553,7 +6541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>227</v>
       </c>
@@ -6589,7 +6577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>62</v>
       </c>
@@ -6631,7 +6619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>230</v>
       </c>
@@ -6667,7 +6655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>63</v>
       </c>
@@ -6709,7 +6697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>233</v>
       </c>
@@ -6745,7 +6733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>64</v>
       </c>
@@ -6787,7 +6775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>237</v>
       </c>
@@ -6823,7 +6811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
         <v>65</v>
       </c>
@@ -6865,7 +6853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>242</v>
       </c>
@@ -6901,7 +6889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="5">
         <v>66</v>
       </c>
@@ -6979,7 +6967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="5">
         <v>67</v>
       </c>
@@ -7021,7 +7009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>249</v>
       </c>
@@ -7063,7 +7051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="5">
         <v>68</v>
       </c>
@@ -7105,7 +7093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>254</v>
       </c>
@@ -7141,7 +7129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" s="5">
         <v>69</v>
       </c>
@@ -7183,7 +7171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>257</v>
       </c>
@@ -7225,7 +7213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" s="5">
         <v>70</v>
       </c>
@@ -7267,7 +7255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>263</v>
       </c>
@@ -7309,7 +7297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" s="5">
         <v>71</v>
       </c>
@@ -7351,7 +7339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>268</v>
       </c>
@@ -7390,7 +7378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" s="5">
         <v>72</v>
       </c>
@@ -7432,7 +7420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>271</v>
       </c>
@@ -7471,7 +7459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" s="5">
         <v>73</v>
       </c>
@@ -7513,7 +7501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>274</v>
       </c>
@@ -7549,7 +7537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" s="5">
         <v>74</v>
       </c>
@@ -7591,7 +7579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>278</v>
       </c>
@@ -7627,7 +7615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" s="5">
         <v>75</v>
       </c>
@@ -7705,7 +7693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" s="5">
         <v>76</v>
       </c>
@@ -7747,7 +7735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>282</v>
       </c>
@@ -7786,7 +7774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" s="5">
         <v>77</v>
       </c>
@@ -7828,7 +7816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>284</v>
       </c>
@@ -7864,7 +7852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" s="5">
         <v>78</v>
       </c>
@@ -7906,7 +7894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>286</v>
       </c>
@@ -7942,7 +7930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" s="5">
         <v>79</v>
       </c>
@@ -7984,7 +7972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>289</v>
       </c>
@@ -8020,7 +8008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" s="5">
         <v>80</v>
       </c>
@@ -8098,7 +8086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" s="5">
         <v>81</v>
       </c>
@@ -8176,7 +8164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" s="5">
         <v>82</v>
       </c>
@@ -8254,7 +8242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" s="5">
         <v>83</v>
       </c>
@@ -8296,7 +8284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>299</v>
       </c>
@@ -8332,7 +8320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" s="5">
         <v>84</v>
       </c>
@@ -8413,7 +8401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" s="5">
         <v>85</v>
       </c>
@@ -8494,7 +8482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" s="5">
         <v>86</v>
       </c>
@@ -8536,7 +8524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>309</v>
       </c>
@@ -8575,7 +8563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" s="5">
         <v>87</v>
       </c>
@@ -8617,7 +8605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>312</v>
       </c>
@@ -8656,7 +8644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" s="5">
         <v>88</v>
       </c>
@@ -8698,7 +8686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>314</v>
       </c>
@@ -8734,7 +8722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" s="5">
         <v>89</v>
       </c>
@@ -8812,7 +8800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" s="5">
         <v>90</v>
       </c>
@@ -8854,7 +8842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
         <v>319</v>
       </c>
@@ -8893,7 +8881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" s="5">
         <v>91</v>
       </c>
@@ -8974,7 +8962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" s="5">
         <v>92</v>
       </c>
@@ -9016,7 +9004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
         <v>325</v>
       </c>
@@ -9052,7 +9040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" s="5">
         <v>93</v>
       </c>
@@ -9130,7 +9118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188" s="5">
         <v>94</v>
       </c>
@@ -9211,7 +9199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190" s="5">
         <v>95</v>
       </c>
@@ -9253,7 +9241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
         <v>332</v>
       </c>
@@ -9289,7 +9277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192" s="5">
         <v>96</v>
       </c>
@@ -9331,7 +9319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
         <v>334</v>
       </c>
@@ -9370,7 +9358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" s="5">
         <v>97</v>
       </c>
@@ -9454,7 +9442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" s="5">
         <v>98</v>
       </c>
@@ -9496,7 +9484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
         <v>343</v>
       </c>
@@ -9532,7 +9520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198" s="5">
         <v>99</v>
       </c>
@@ -9543,10 +9531,10 @@
         <v>204</v>
       </c>
       <c r="D198" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E198" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F198" t="s">
         <v>15</v>
@@ -9575,25 +9563,25 @@
       </c>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A199" s="6" t="s">
+      <c r="A199" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="B199" s="6">
+      <c r="B199" s="3">
         <v>2</v>
       </c>
-      <c r="C199" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="D199" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E199" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F199" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G199" s="7" t="s">
+      <c r="C199" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D199" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E199" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F199" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G199" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H199" t="s">
@@ -9610,7 +9598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" s="5">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
New LLaVA Trials I did over the last few weeks
</commit_message>
<xml_diff>
--- a/llava-trials.xlsx
+++ b/llava-trials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryana\OneDrive\Documents\Actual Documents\extracted_frames_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32D50D8-5FFF-45DB-9D9F-77D3C9BE0AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2186637-CE14-477E-9119-D2EEED8C47B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{AD63279E-0698-49CC-BCD4-922352F5CF60}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AD63279E-0698-49CC-BCD4-922352F5CF60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1726,8 +1726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F41316-F566-4B06-BB05-B7BBB865FBE7}">
   <dimension ref="A1:M213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="N180" sqref="N180"/>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="G129" sqref="G129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6474,7 +6474,7 @@
         <v>141</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E121" s="4" t="s">
         <v>14</v>
@@ -9609,10 +9609,10 @@
         <v>234</v>
       </c>
       <c r="D200" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E200" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F200" t="s">
         <v>15</v>
@@ -9641,25 +9641,25 @@
       </c>
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A201" s="6" t="s">
+      <c r="A201" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="B201" s="6">
+      <c r="B201" s="3">
         <v>2</v>
       </c>
-      <c r="C201" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="D201" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E201" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F201" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G201" s="7" t="s">
+      <c r="C201" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D201" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E201" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F201" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G201" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H201" t="s">
@@ -9709,7 +9709,7 @@
         <v>354</v>
       </c>
       <c r="B209" s="10">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
@@ -9733,7 +9733,7 @@
         <v>357</v>
       </c>
       <c r="B212" s="10">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>